<commit_message>
Twitter Post and Posts Tweet Replies API
</commit_message>
<xml_diff>
--- a/Notebooks/data/MIND.xlsx
+++ b/Notebooks/data/MIND.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="934">
   <si>
     <t>Profile URL</t>
   </si>
@@ -2810,13 +2810,16 @@
   </si>
   <si>
     <t>https://x.com/jbondwagon</t>
+  </si>
+  <si>
+    <t>https://x.com/adekvat276</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2827,6 +2830,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -2847,7 +2854,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2855,6 +2862,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -9027,7 +9037,7 @@
       <c r="A745" s="1">
         <v>744.0</v>
       </c>
-      <c r="B745" s="2" t="s">
+      <c r="B745" s="3" t="s">
         <v>744</v>
       </c>
     </row>
@@ -10531,8 +10541,16 @@
       <c r="A933" s="1">
         <v>933.0</v>
       </c>
-      <c r="B933" s="2" t="s">
+      <c r="B933" s="3" t="s">
         <v>932</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="1">
+        <v>934.0</v>
+      </c>
+      <c r="B934" s="3" t="s">
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -11469,10 +11487,11 @@
     <hyperlink r:id="rId930" ref="B931"/>
     <hyperlink r:id="rId931" ref="B932"/>
     <hyperlink r:id="rId932" ref="B933"/>
+    <hyperlink r:id="rId933" ref="B934"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId933"/>
+  <drawing r:id="rId934"/>
 </worksheet>
 </file>
</xml_diff>